<commit_message>
Added background image to minigame - not the correct size in game atm
</commit_message>
<xml_diff>
--- a/desktop/out/production/resources/Data/yorkMap.xlsx
+++ b/desktop/out/production/resources/Data/yorkMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\warKroy\core\src\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\Work\SEPR\Assessment 3\Code\Septagon3\core\assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D437A9-69FB-47B0-AFFE-0109E8AC2196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9666481-89F6-40C1-9964-25EBB9D8BDBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="27555" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yorkMap" sheetId="1" r:id="rId1"/>
@@ -546,17 +546,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="111">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="38">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -574,510 +564,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1673,12 +1159,12 @@
       <selection activeCell="BR11" sqref="BR11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="71" width="2.5703125" customWidth="1"/>
+    <col min="1" max="71" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1872,7 +1358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2066,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2260,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2454,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2648,7 +2134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2842,7 +2328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3036,7 +2522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3230,7 +2716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3424,7 +2910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3618,7 +3104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -3812,7 +3298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -4006,7 +3492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -4200,7 +3686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -4394,7 +3880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4588,7 +4074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4782,7 +4268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -4976,7 +4462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -5170,7 +4656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -5364,7 +4850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -5558,7 +5044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -5752,7 +5238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -5946,7 +5432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -6140,7 +5626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -6334,7 +5820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -6528,7 +6014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -6722,7 +6208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -6916,7 +6402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -7110,7 +6596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -7304,7 +6790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -7498,7 +6984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -7692,7 +7178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -7886,7 +7372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -8080,7 +7566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -8274,7 +7760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -8468,7 +7954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3</v>
       </c>
@@ -8664,136 +8150,136 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A38:BR38 A1:AT1 A30:BK36 A5:BH18 A19:AY23 A24:AZ24 A27:BF29 A25:BD26 BL33:BL36 AY4:BH4 AY3:BL3 AO3:AP4 AO2:AT2 A2:AE4">
-    <cfRule type="cellIs" dxfId="74" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:BL2">
-    <cfRule type="cellIs" dxfId="70" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI4:BL18">
-    <cfRule type="cellIs" dxfId="66" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ19:BL23">
-    <cfRule type="cellIs" dxfId="62" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA24:BL24">
-    <cfRule type="cellIs" dxfId="58" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG25:BL29 BL30:BL32">
-    <cfRule type="cellIs" dxfId="54" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE25:BF26">
-    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ3:AX4">
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF2:AN4">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:BL36">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>